<commit_message>
Unit tests for column width and row height
</commit_message>
<xml_diff>
--- a/tests/data/Reader/XLSX/rowColumnAttributeTest.xlsx
+++ b/tests/data/Reader/XLSX/rowColumnAttributeTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PHPSpreadsheet\develop\tests\data\Reader\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149FF73B-D140-44FA-90FD-5E8316B74929}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D1A5BA-10A6-42C8-BBDC-BAAE87EE4122}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5123" yWindow="765" windowWidth="22830" windowHeight="13237" xr2:uid="{C246BD48-C462-408F-A36E-981D8ADF7BF5}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -51,6 +51,33 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -405,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC73DCA-3B43-4E06-BA19-6DBEBEA12E06}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F1" sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -417,9 +444,10 @@
     <col min="2" max="2" width="6.59765625" customWidth="1"/>
     <col min="3" max="3" width="8.59765625" customWidth="1"/>
     <col min="4" max="4" width="10.59765625" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -432,8 +460,12 @@
       <c r="D1" s="1">
         <v>4</v>
       </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>5</v>
       </c>
@@ -446,8 +478,12 @@
       <c r="D2" s="1">
         <v>8</v>
       </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>9</v>
       </c>
@@ -460,8 +496,12 @@
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -473,6 +513,36 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>